<commit_message>
Updated the script in MobileSettings page
</commit_message>
<xml_diff>
--- a/tests/artifact/data/Mobile-Settings.data.xlsx
+++ b/tests/artifact/data/Mobile-Settings.data.xlsx
@@ -4,17 +4,30 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950"/>
+    <workbookView windowWidth="18350" windowHeight="6800"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="255">
   <si>
     <r>
       <rPr>
@@ -178,10 +191,16 @@
     <t>//select[@id="gs-t2-select-30"]</t>
   </si>
   <si>
+    <t>org.Transaction.NegativeStock</t>
+  </si>
+  <si>
+    <t>(//input[@type="checkbox"])[1]</t>
+  </si>
+  <si>
     <t>org.Transaction.TrackTransaction</t>
   </si>
   <si>
-    <t>//input[@type="checkbox"]</t>
+    <t>(//input[@type="checkbox"])[2]</t>
   </si>
   <si>
     <t>Org.ImportData</t>
@@ -637,13 +656,13 @@
     <t>GSTINValidate.Form</t>
   </si>
   <si>
-    <t>//h5[@id="gstin-validation-modal___BV_modal_title_"]</t>
+    <t>//h5[text()='GSTIN Validation']</t>
   </si>
   <si>
     <t>ValidateButton.Close</t>
   </si>
   <si>
-    <t>//button[text()='×']</t>
+    <t>//button[text()=' x']</t>
   </si>
   <si>
     <t>Organization.PAN</t>
@@ -787,7 +806,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
@@ -2116,10 +2135,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C130"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="B91" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>
@@ -2350,7 +2369,7 @@
       <c r="A28" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="9" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2410,7 +2429,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" ht="16" spans="1:2">
+    <row r="36" s="1" customFormat="1" ht="23.1" customHeight="1" spans="1:2">
       <c r="A36" s="4" t="s">
         <v>67</v>
       </c>
@@ -2434,11 +2453,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" s="1" customFormat="1" ht="23.1" customHeight="1" spans="1:2">
+    <row r="39" ht="16" spans="1:2">
       <c r="A39" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="8" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2446,15 +2465,15 @@
       <c r="A40" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="41" s="3" customFormat="1" ht="16" spans="1:2">
+    <row r="41" s="1" customFormat="1" ht="23.1" customHeight="1" spans="1:2">
       <c r="A41" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="8" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2594,11 +2613,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="59" ht="15.5" spans="1:2">
+    <row r="59" s="3" customFormat="1" ht="16" spans="1:2">
       <c r="A59" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="3" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2642,15 +2661,15 @@
         <v>124</v>
       </c>
     </row>
-    <row r="65" ht="16" spans="1:2">
+    <row r="65" ht="15.5" spans="1:2">
       <c r="A65" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="66" s="1" customFormat="1" ht="23.1" customHeight="1" spans="1:2">
+    <row r="66" ht="16" spans="1:2">
       <c r="A66" s="4" t="s">
         <v>127</v>
       </c>
@@ -2658,11 +2677,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" ht="15.5" spans="1:2">
+    <row r="67" s="1" customFormat="1" ht="23.1" customHeight="1" spans="1:2">
       <c r="A67" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="8" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2763,7 +2782,7 @@
       </c>
     </row>
     <row r="80" ht="15.5" spans="1:2">
-      <c r="A80" s="12" t="s">
+      <c r="A80" s="4" t="s">
         <v>155</v>
       </c>
       <c r="B80" t="s">
@@ -2778,19 +2797,19 @@
         <v>158</v>
       </c>
     </row>
-    <row r="82" ht="16" spans="1:2">
+    <row r="82" ht="15.5" spans="1:2">
       <c r="A82" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="B82" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="83" ht="15.5" spans="1:2">
-      <c r="A83" s="4" t="s">
+    <row r="83" ht="16" spans="1:2">
+      <c r="A83" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="8" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2803,7 +2822,7 @@
       </c>
     </row>
     <row r="85" ht="15.5" spans="1:2">
-      <c r="A85" s="12" t="s">
+      <c r="A85" s="4" t="s">
         <v>165</v>
       </c>
       <c r="B85" t="s">
@@ -2822,7 +2841,7 @@
       <c r="A87" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="B87" s="13" t="s">
+      <c r="B87" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2830,7 +2849,7 @@
       <c r="A88" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="13" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3111,15 +3130,15 @@
         <v>241</v>
       </c>
       <c r="B123" t="s">
-        <v>142</v>
+        <v>242</v>
       </c>
     </row>
     <row r="124" ht="15.5" spans="1:2">
       <c r="A124" s="12" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B124" t="s">
-        <v>243</v>
+        <v>144</v>
       </c>
     </row>
     <row r="125" ht="15.5" spans="1:2">
@@ -3135,39 +3154,47 @@
         <v>246</v>
       </c>
       <c r="B126" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
     </row>
     <row r="127" ht="15.5" spans="1:2">
       <c r="A127" s="12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B127" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="128" ht="15.5" spans="1:2">
-      <c r="A128" s="4" t="s">
-        <v>248</v>
+      <c r="A128" s="12" t="s">
+        <v>249</v>
       </c>
       <c r="B128" t="s">
-        <v>14</v>
+        <v>236</v>
       </c>
     </row>
     <row r="129" ht="15.5" spans="1:2">
       <c r="A129" s="4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B129" t="s">
-        <v>250</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" ht="15.5" spans="1:2">
       <c r="A130" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="B130" s="10" t="s">
+      <c r="B130" t="s">
         <v>252</v>
+      </c>
+    </row>
+    <row r="131" ht="15.5" spans="1:2">
+      <c r="A131" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B131" s="10" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -3339,466 +3366,436 @@
       <formula>LEN(TRIM(C26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="beginsWith" dxfId="3" priority="181" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A27,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="182" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A27,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="183" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A27,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="184" stopIfTrue="1">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="4" priority="129" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="130">
-      <formula>LEN(TRIM(B27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27:E27">
-    <cfRule type="expression" dxfId="4" priority="185" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="186">
-      <formula>LEN(TRIM(C27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
+  <conditionalFormatting sqref="A29">
     <cfRule type="beginsWith" dxfId="3" priority="175" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A28,LEN("//"))="//"</formula>
+      <formula>LEFT(A29,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="176" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A28,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A29,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="177" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A28,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A29,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="178" stopIfTrue="1">
-      <formula>LEN(TRIM(A28))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B28:E28">
+      <formula>LEN(TRIM(A29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29:E29">
     <cfRule type="expression" dxfId="4" priority="179" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="180">
-      <formula>LEN(TRIM(B28))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
+      <formula>LEN(TRIM(B29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
     <cfRule type="expression" dxfId="4" priority="171" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="172">
-      <formula>LEN(TRIM(B29))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
+      <formula>LEN(TRIM(B30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
     <cfRule type="beginsWith" dxfId="3" priority="165" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A32,LEN("//"))="//"</formula>
+      <formula>LEFT(A33,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="166" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A32,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A33,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="167" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A32,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A33,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="168" stopIfTrue="1">
-      <formula>LEN(TRIM(A32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B32:E32">
+      <formula>LEN(TRIM(A33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33:E33">
     <cfRule type="expression" dxfId="4" priority="169" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="170">
-      <formula>LEN(TRIM(B32))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
+      <formula>LEN(TRIM(B33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
     <cfRule type="beginsWith" dxfId="3" priority="161" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A33,LEN("//"))="//"</formula>
+      <formula>LEFT(A34,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="162" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A33,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A34,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="163" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A33,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A34,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="164" stopIfTrue="1">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
     <cfRule type="beginsWith" dxfId="3" priority="155" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A34,LEN("//"))="//"</formula>
+      <formula>LEFT(A35,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="156" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A34,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A35,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="157" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A34,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A35,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="158" stopIfTrue="1">
-      <formula>LEN(TRIM(A34))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B34:E34">
+      <formula>LEN(TRIM(A35))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35:E35">
     <cfRule type="expression" dxfId="4" priority="159" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="160">
-      <formula>LEN(TRIM(B34))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
+      <formula>LEN(TRIM(B35))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
     <cfRule type="beginsWith" dxfId="3" priority="149" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A35,LEN("//"))="//"</formula>
+      <formula>LEFT(A36,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="150" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A35,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A36,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="151" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A35,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A36,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="152" stopIfTrue="1">
-      <formula>LEN(TRIM(A35))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B35:E35">
+      <formula>LEN(TRIM(A36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36:E36">
     <cfRule type="expression" dxfId="4" priority="153" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="154">
-      <formula>LEN(TRIM(B35))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
+      <formula>LEN(TRIM(B36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
     <cfRule type="beginsWith" dxfId="3" priority="145" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A36,LEN("//"))="//"</formula>
+      <formula>LEFT(A37,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="146" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A36,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A37,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="147" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A36,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A37,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="148" stopIfTrue="1">
-      <formula>LEN(TRIM(A36))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B36">
+      <formula>LEN(TRIM(A37))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37">
     <cfRule type="expression" dxfId="4" priority="251" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="252">
-      <formula>LEN(TRIM(B36))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
+      <formula>LEN(TRIM(B37))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
     <cfRule type="beginsWith" dxfId="3" priority="141" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A37,LEN("//"))="//"</formula>
+      <formula>LEFT(A38,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="142" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A37,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A38,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="143" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A37,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A38,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="144" stopIfTrue="1">
-      <formula>LEN(TRIM(A37))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B37">
+      <formula>LEN(TRIM(A38))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38">
     <cfRule type="expression" dxfId="4" priority="245" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="246">
-      <formula>LEN(TRIM(B37))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
+      <formula>LEN(TRIM(B38))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39">
     <cfRule type="beginsWith" dxfId="3" priority="137" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A38,LEN("//"))="//"</formula>
+      <formula>LEFT(A39,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="138" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A38,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A39,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="139" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A38,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A39,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="140" stopIfTrue="1">
-      <formula>LEN(TRIM(A38))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B38">
+      <formula>LEN(TRIM(A39))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39">
     <cfRule type="expression" dxfId="4" priority="239" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="240">
-      <formula>LEN(TRIM(B38))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
+      <formula>LEN(TRIM(B39))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43">
     <cfRule type="beginsWith" dxfId="3" priority="133" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A42,LEN("//"))="//"</formula>
+      <formula>LEFT(A43,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="134" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A42,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A43,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="135" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A42,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A43,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="136" stopIfTrue="1">
-      <formula>LEN(TRIM(A42))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
+      <formula>LEN(TRIM(A43))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
     <cfRule type="beginsWith" dxfId="3" priority="217" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A58,LEN("//"))="//"</formula>
+      <formula>LEFT(A59,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="218" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A58,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A59,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="219" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A58,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A59,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="220" stopIfTrue="1">
-      <formula>LEN(TRIM(A58))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65">
+      <formula>LEN(TRIM(A59))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66">
     <cfRule type="beginsWith" dxfId="3" priority="119" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A65,LEN("//"))="//"</formula>
+      <formula>LEFT(A66,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="120" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A65,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A66,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="121" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A65,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A66,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="122" stopIfTrue="1">
-      <formula>LEN(TRIM(A65))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B65">
+      <formula>LEN(TRIM(A66))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B66">
     <cfRule type="expression" dxfId="4" priority="123" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="124">
-      <formula>LEN(TRIM(B65))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A66">
+      <formula>LEN(TRIM(B66))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
     <cfRule type="beginsWith" dxfId="3" priority="113" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A66,LEN("//"))="//"</formula>
+      <formula>LEFT(A67,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="114" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A66,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A67,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="115" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A66,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A67,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="116" stopIfTrue="1">
-      <formula>LEN(TRIM(A66))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B66">
+      <formula>LEN(TRIM(A67))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B67">
     <cfRule type="expression" dxfId="4" priority="111" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="112">
-      <formula>LEN(TRIM(B66))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C66:E66">
+      <formula>LEN(TRIM(B67))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67:E67">
     <cfRule type="expression" dxfId="4" priority="117" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="118">
-      <formula>LEN(TRIM(C66))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71">
+      <formula>LEN(TRIM(C67))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A72">
     <cfRule type="beginsWith" dxfId="3" priority="103" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A71,LEN("//"))="//"</formula>
+      <formula>LEFT(A72,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="104" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A71,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A72,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="105" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A71,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A72,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="106" stopIfTrue="1">
-      <formula>LEN(TRIM(A71))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
+      <formula>LEN(TRIM(A72))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A73">
     <cfRule type="beginsWith" dxfId="3" priority="99" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A72,LEN("//"))="//"</formula>
+      <formula>LEFT(A73,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="100" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A72,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A73,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="101" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A72,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A73,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="102" stopIfTrue="1">
-      <formula>LEN(TRIM(A72))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A75">
+      <formula>LEN(TRIM(A73))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A76">
     <cfRule type="beginsWith" dxfId="3" priority="91" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A75,LEN("//"))="//"</formula>
+      <formula>LEFT(A76,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="92" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A75,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A76,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="93" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A75,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A76,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="94" stopIfTrue="1">
-      <formula>LEN(TRIM(A75))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B82">
+      <formula>LEN(TRIM(A76))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83">
     <cfRule type="expression" dxfId="4" priority="65" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="66">
-      <formula>LEN(TRIM(B82))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A84">
+      <formula>LEN(TRIM(B83))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A85">
     <cfRule type="beginsWith" dxfId="3" priority="13" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A84,LEN("//"))="//"</formula>
+      <formula>LEFT(A85,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="14" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A84,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A85,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="15" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A84,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A85,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="16" stopIfTrue="1">
-      <formula>LEN(TRIM(A84))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A113">
+      <formula>LEN(TRIM(A85))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A114">
     <cfRule type="beginsWith" dxfId="3" priority="25" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A113,LEN("//"))="//"</formula>
+      <formula>LEFT(A114,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="26" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A113,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A114,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="27" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A113,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A114,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="28" stopIfTrue="1">
-      <formula>LEN(TRIM(A113))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A120">
+      <formula>LEN(TRIM(A114))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A121">
     <cfRule type="beginsWith" dxfId="3" priority="17" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A120,LEN("//"))="//"</formula>
+      <formula>LEFT(A121,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="18" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A120,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A121,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="19" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A120,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A121,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="20" stopIfTrue="1">
-      <formula>LEN(TRIM(A120))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A123">
+      <formula>LEN(TRIM(A121))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A124">
     <cfRule type="beginsWith" dxfId="3" priority="57" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A123,LEN("//"))="//"</formula>
+      <formula>LEFT(A124,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="58" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A123,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A124,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="59" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A123,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A124,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="60" stopIfTrue="1">
-      <formula>LEN(TRIM(A123))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A126">
+      <formula>LEN(TRIM(A124))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A127">
     <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A126,LEN("//"))="//"</formula>
+      <formula>LEFT(A127,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A126,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A127,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A126,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A127,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
-      <formula>LEN(TRIM(A126))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A127">
+      <formula>LEN(TRIM(A127))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A128">
     <cfRule type="beginsWith" dxfId="3" priority="53" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A127,LEN("//"))="//"</formula>
+      <formula>LEFT(A128,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="54" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A127,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A128,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="55" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A127,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A128,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="56" stopIfTrue="1">
-      <formula>LEN(TRIM(A127))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A128">
+      <formula>LEN(TRIM(A128))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A129">
     <cfRule type="beginsWith" dxfId="3" priority="45" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A128,LEN("//"))="//"</formula>
+      <formula>LEFT(A129,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="46" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A128,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A129,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="47" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A128,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A129,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="48" stopIfTrue="1">
-      <formula>LEN(TRIM(A128))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A129">
+      <formula>LEN(TRIM(A129))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A130">
     <cfRule type="beginsWith" dxfId="3" priority="9" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A129,LEN("//"))="//"</formula>
+      <formula>LEFT(A130,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="10" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A129,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A130,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="11" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A129,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A130,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="12" stopIfTrue="1">
-      <formula>LEN(TRIM(A129))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A130">
+      <formula>LEN(TRIM(A130))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A131">
     <cfRule type="beginsWith" dxfId="3" priority="5" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A130,LEN("//"))="//"</formula>
+      <formula>LEFT(A131,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="6" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A130,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A131,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="7" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A130,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A131,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="8" stopIfTrue="1">
-      <formula>LEN(TRIM(A130))&gt;0</formula>
+      <formula>LEN(TRIM(A131))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A9">
@@ -3843,144 +3840,158 @@
       <formula>LEN(TRIM(A19))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A29:A31">
+  <conditionalFormatting sqref="A27:A28">
+    <cfRule type="beginsWith" dxfId="3" priority="181" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A27,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="182" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A27,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="183" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A27,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="184" stopIfTrue="1">
+      <formula>LEN(TRIM(A27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30:A32">
     <cfRule type="beginsWith" dxfId="3" priority="271" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A29,LEN("//"))="//"</formula>
+      <formula>LEFT(A30,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="272" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A29,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A30,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="273" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A29,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A30,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="274" stopIfTrue="1">
-      <formula>LEN(TRIM(A29))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A39:A40">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:A41">
     <cfRule type="beginsWith" dxfId="3" priority="231" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A39,LEN("//"))="//"</formula>
+      <formula>LEFT(A40,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="232" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A39,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A40,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="233" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A39,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A40,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="234" stopIfTrue="1">
-      <formula>LEN(TRIM(A39))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59:A60">
+      <formula>LEN(TRIM(A40))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:A61">
     <cfRule type="beginsWith" dxfId="3" priority="213" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A59,LEN("//"))="//"</formula>
+      <formula>LEFT(A60,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="214" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A59,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A60,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="215" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A59,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A60,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="216" stopIfTrue="1">
-      <formula>LEN(TRIM(A59))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67:A70">
+      <formula>LEN(TRIM(A60))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:A71">
     <cfRule type="beginsWith" dxfId="3" priority="107" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A67,LEN("//"))="//"</formula>
+      <formula>LEFT(A68,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="108" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A67,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A68,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="109" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A67,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A68,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="110" stopIfTrue="1">
-      <formula>LEN(TRIM(A67))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A73:A74">
+      <formula>LEN(TRIM(A68))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A74:A75">
     <cfRule type="beginsWith" dxfId="3" priority="95" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A73,LEN("//"))="//"</formula>
+      <formula>LEFT(A74,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="96" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A73,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A74,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="97" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A73,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A74,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="98" stopIfTrue="1">
-      <formula>LEN(TRIM(A73))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A76:A80">
+      <formula>LEN(TRIM(A74))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A77:A81">
     <cfRule type="beginsWith" dxfId="3" priority="79" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A76,LEN("//"))="//"</formula>
+      <formula>LEFT(A77,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="80" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A76,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A77,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="81" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A76,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A77,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="82" stopIfTrue="1">
-      <formula>LEN(TRIM(A76))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A81:A82">
+      <formula>LEN(TRIM(A77))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82:A83">
     <cfRule type="beginsWith" dxfId="3" priority="71" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A81,LEN("//"))="//"</formula>
+      <formula>LEFT(A82,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="72" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A81,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A82,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="73" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A81,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A82,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="74" stopIfTrue="1">
-      <formula>LEN(TRIM(A81))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A114:A115">
+      <formula>LEN(TRIM(A82))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A115:A116">
     <cfRule type="beginsWith" dxfId="3" priority="21" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A114,LEN("//"))="//"</formula>
+      <formula>LEFT(A115,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="22" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A114,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A115,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="23" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A114,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A115,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="24" stopIfTrue="1">
-      <formula>LEN(TRIM(A114))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A121:A122">
+      <formula>LEN(TRIM(A115))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A122:A123">
     <cfRule type="beginsWith" dxfId="3" priority="61" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A121,LEN("//"))="//"</formula>
+      <formula>LEFT(A122,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="62" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A121,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A122,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="63" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A121,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A122,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="64" stopIfTrue="1">
-      <formula>LEN(TRIM(A121))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A124:A125">
+      <formula>LEN(TRIM(A122))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A125:A126">
     <cfRule type="beginsWith" dxfId="3" priority="49" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A124,LEN("//"))="//"</formula>
+      <formula>LEFT(A125,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="50" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A124,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A125,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="51" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A124,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A125,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="52" stopIfTrue="1">
-      <formula>LEN(TRIM(A124))&gt;0</formula>
+      <formula>LEN(TRIM(A125))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B9">
@@ -4007,12 +4018,20 @@
       <formula>LEN(TRIM(B22))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39:B40">
+  <conditionalFormatting sqref="B27:B28">
+    <cfRule type="expression" dxfId="4" priority="129" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="130">
+      <formula>LEN(TRIM(B27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40:B41">
     <cfRule type="expression" dxfId="4" priority="235" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="236">
-      <formula>LEN(TRIM(B39))&gt;0</formula>
+      <formula>LEN(TRIM(B40))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:E9">
@@ -4061,62 +4080,70 @@
       <formula>LEN(TRIM(C22))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:E29 B30:E31 B33:E33">
+  <conditionalFormatting sqref="C27:E28">
+    <cfRule type="expression" dxfId="4" priority="185" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="186">
+      <formula>LEN(TRIM(C27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30:E30 B34:E34 B31:E32">
     <cfRule type="expression" dxfId="4" priority="275" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="276">
-      <formula>LEN(TRIM(B29))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C39:E40">
+      <formula>LEN(TRIM(B30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40:E41">
     <cfRule type="expression" dxfId="4" priority="237" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="5" priority="238">
-      <formula>LEN(TRIM(C39))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41 A43:A57">
+      <formula>LEN(TRIM(C40))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42 A44:A58">
     <cfRule type="beginsWith" dxfId="3" priority="221" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A41,LEN("//"))="//"</formula>
+      <formula>LEFT(A42,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="222" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A41,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A42,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="223" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A41,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A42,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="224" stopIfTrue="1">
-      <formula>LEN(TRIM(A41))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61:A64 A83">
+      <formula>LEN(TRIM(A42))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:A65 A84">
     <cfRule type="beginsWith" dxfId="3" priority="125" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A61,LEN("//"))="//"</formula>
+      <formula>LEFT(A62,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="126" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A61,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A62,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="127" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A61,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A62,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="128" stopIfTrue="1">
-      <formula>LEN(TRIM(A61))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A85:A112 A116:A119">
+      <formula>LEN(TRIM(A62))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A86:A113 A117:A120">
     <cfRule type="beginsWith" dxfId="3" priority="67" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A85,LEN("//"))="//"</formula>
+      <formula>LEFT(A86,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="68" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A85,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A86,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="69" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A85,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A86,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="70" stopIfTrue="1">
-      <formula>LEN(TRIM(A85))&gt;0</formula>
+      <formula>LEN(TRIM(A86))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>